<commit_message>
fixed bug in test.py
</commit_message>
<xml_diff>
--- a/spot_auction_results/spot_data.xlsx
+++ b/spot_auction_results/spot_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jens/Documents/Python/dynprog/spot_auction_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD63E6D6-0933-7740-A4BA-0994335D3CDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC7E033-13F8-AC41-9692-A73E792521E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="460" windowWidth="21320" windowHeight="17100" xr2:uid="{97F7539C-452B-A548-92BB-3CE594F78CD0}"/>
   </bookViews>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Time</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Price CH</t>
   </si>
@@ -3585,29 +3582,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2513C063-BB01-5E4E-BC20-809D3836ED8C}">
-  <dimension ref="A1:D289"/>
+  <dimension ref="A1:D313"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F288" sqref="F288"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3640,7 +3631,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>43935.08333321759</v>
+        <v>43935.083333333336</v>
       </c>
       <c r="B4">
         <v>8.0500000000000007</v>
@@ -3654,7 +3645,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>43935.124999826388</v>
+        <v>43935.125</v>
       </c>
       <c r="B5">
         <v>8.6</v>
@@ -3668,7 +3659,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>43935.166666435187</v>
+        <v>43935.166666666664</v>
       </c>
       <c r="B6">
         <v>10.02</v>
@@ -3682,7 +3673,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>43935.208333043978</v>
+        <v>43935.208333333336</v>
       </c>
       <c r="B7">
         <v>13.32</v>
@@ -3696,7 +3687,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>43935.249999652777</v>
+        <v>43935.25</v>
       </c>
       <c r="B8">
         <v>23.66</v>
@@ -3710,7 +3701,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>43935.291666261575</v>
+        <v>43935.291666666664</v>
       </c>
       <c r="B9">
         <v>24.7</v>
@@ -3724,7 +3715,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>43935.333332870374</v>
+        <v>43935.333333333336</v>
       </c>
       <c r="B10">
         <v>24.73</v>
@@ -3738,7 +3729,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>43935.374999479165</v>
+        <v>43935.375</v>
       </c>
       <c r="B11">
         <v>23.73</v>
@@ -3752,7 +3743,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>43935.416666087964</v>
+        <v>43935.416666666664</v>
       </c>
       <c r="B12">
         <v>21.05</v>
@@ -3766,7 +3757,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>43935.458332696762</v>
+        <v>43935.458333333336</v>
       </c>
       <c r="B13">
         <v>18.37</v>
@@ -3780,7 +3771,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>43935.499999305554</v>
+        <v>43935.5</v>
       </c>
       <c r="B14">
         <v>16.170000000000002</v>
@@ -3794,7 +3785,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>43935.541665914352</v>
+        <v>43935.541666666664</v>
       </c>
       <c r="B15">
         <v>15.52</v>
@@ -3808,7 +3799,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>43935.583332523151</v>
+        <v>43935.583333333336</v>
       </c>
       <c r="B16">
         <v>14.31</v>
@@ -3822,7 +3813,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>43935.624999131942</v>
+        <v>43935.625</v>
       </c>
       <c r="B17">
         <v>15.41</v>
@@ -3836,7 +3827,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>43935.66666574074</v>
+        <v>43935.666666666664</v>
       </c>
       <c r="B18">
         <v>18.22</v>
@@ -3850,7 +3841,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>43935.708332349539</v>
+        <v>43935.708333333336</v>
       </c>
       <c r="B19">
         <v>22.5</v>
@@ -3864,7 +3855,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>43935.74999895833</v>
+        <v>43935.75</v>
       </c>
       <c r="B20">
         <v>25.83</v>
@@ -3878,7 +3869,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>43935.791665567129</v>
+        <v>43935.791666666664</v>
       </c>
       <c r="B21">
         <v>26.06</v>
@@ -3892,7 +3883,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>43935.833332175927</v>
+        <v>43935.833333333336</v>
       </c>
       <c r="B22">
         <v>27.66</v>
@@ -3906,7 +3897,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>43935.874998784719</v>
+        <v>43935.875</v>
       </c>
       <c r="B23">
         <v>27.76</v>
@@ -3920,7 +3911,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>43935.916665393517</v>
+        <v>43935.916666666664</v>
       </c>
       <c r="B24">
         <v>25.39</v>
@@ -3934,7 +3925,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>43935.958332002316</v>
+        <v>43935.958333333336</v>
       </c>
       <c r="B25">
         <v>22.16</v>
@@ -3948,7 +3939,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>43935.999998611114</v>
+        <v>43936</v>
       </c>
       <c r="B26">
         <v>20.63</v>
@@ -3962,7 +3953,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>43936.041665219906</v>
+        <v>43936.041666666664</v>
       </c>
       <c r="B27">
         <v>19.05</v>
@@ -3976,7 +3967,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>43936.083331828704</v>
+        <v>43936.083333333336</v>
       </c>
       <c r="B28">
         <v>17.5</v>
@@ -3990,7 +3981,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>43936.124998437503</v>
+        <v>43936.125</v>
       </c>
       <c r="B29">
         <v>17.190000000000001</v>
@@ -4004,7 +3995,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>43936.166665046294</v>
+        <v>43936.166666666664</v>
       </c>
       <c r="B30">
         <v>17.28</v>
@@ -4018,7 +4009,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>43936.208331655092</v>
+        <v>43936.208333333336</v>
       </c>
       <c r="B31">
         <v>19.940000000000001</v>
@@ -4032,7 +4023,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>43936.249998263891</v>
+        <v>43936.25</v>
       </c>
       <c r="B32">
         <v>25.08</v>
@@ -4046,7 +4037,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>43936.291664872682</v>
+        <v>43936.291666666664</v>
       </c>
       <c r="B33">
         <v>26.16</v>
@@ -4060,7 +4051,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>43936.333331481481</v>
+        <v>43936.333333333336</v>
       </c>
       <c r="B34">
         <v>26.4</v>
@@ -4074,7 +4065,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>43936.374998090279</v>
+        <v>43936.375</v>
       </c>
       <c r="B35">
         <v>19.899999999999999</v>
@@ -4088,7 +4079,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>43936.416664699071</v>
+        <v>43936.416666666664</v>
       </c>
       <c r="B36">
         <v>16.05</v>
@@ -4102,7 +4093,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>43936.458331307869</v>
+        <v>43936.458333333336</v>
       </c>
       <c r="B37">
         <v>12.6</v>
@@ -4116,7 +4107,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>43936.499997916668</v>
+        <v>43936.5</v>
       </c>
       <c r="B38">
         <v>11.23</v>
@@ -4130,7 +4121,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>43936.541664525466</v>
+        <v>43936.541666666664</v>
       </c>
       <c r="B39">
         <v>9.07</v>
@@ -4144,7 +4135,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>43936.583331134258</v>
+        <v>43936.583333333336</v>
       </c>
       <c r="B40">
         <v>7.93</v>
@@ -4158,7 +4149,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>43936.624997743056</v>
+        <v>43936.625</v>
       </c>
       <c r="B41">
         <v>7.65</v>
@@ -4172,7 +4163,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>43936.666664351855</v>
+        <v>43936.666666666664</v>
       </c>
       <c r="B42">
         <v>9.76</v>
@@ -4186,7 +4177,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>43936.708330960646</v>
+        <v>43936.708333333336</v>
       </c>
       <c r="B43">
         <v>20.57</v>
@@ -4200,7 +4191,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>43936.749997569445</v>
+        <v>43936.75</v>
       </c>
       <c r="B44">
         <v>25.7</v>
@@ -4214,7 +4205,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>43936.791664178243</v>
+        <v>43936.791666666664</v>
       </c>
       <c r="B45">
         <v>26.19</v>
@@ -4228,7 +4219,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>43936.833330787034</v>
+        <v>43936.833333333336</v>
       </c>
       <c r="B46">
         <v>27.59</v>
@@ -4242,7 +4233,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>43936.874997395833</v>
+        <v>43936.875</v>
       </c>
       <c r="B47">
         <v>27.08</v>
@@ -4256,7 +4247,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>43936.916664004631</v>
+        <v>43936.916666666664</v>
       </c>
       <c r="B48">
         <v>26.01</v>
@@ -4270,7 +4261,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>43936.958330613423</v>
+        <v>43936.958333333336</v>
       </c>
       <c r="B49">
         <v>23.39</v>
@@ -4284,7 +4275,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>43936.999997222221</v>
+        <v>43937</v>
       </c>
       <c r="B50">
         <v>20.63</v>
@@ -4298,7 +4289,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <v>43937.04166383102</v>
+        <v>43937.041666666664</v>
       </c>
       <c r="B51">
         <v>19.05</v>
@@ -4312,7 +4303,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>43937.083330439818</v>
+        <v>43937.083333333336</v>
       </c>
       <c r="B52">
         <v>17.5</v>
@@ -4326,7 +4317,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>43937.12499704861</v>
+        <v>43937.125</v>
       </c>
       <c r="B53">
         <v>17.190000000000001</v>
@@ -4340,7 +4331,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
-        <v>43937.166663657408</v>
+        <v>43937.166666666664</v>
       </c>
       <c r="B54">
         <v>17.28</v>
@@ -4354,7 +4345,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
-        <v>43937.208330266207</v>
+        <v>43937.208333333336</v>
       </c>
       <c r="B55">
         <v>19.940000000000001</v>
@@ -4368,7 +4359,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <v>43937.249996874998</v>
+        <v>43937.25</v>
       </c>
       <c r="B56">
         <v>25.08</v>
@@ -4382,7 +4373,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
-        <v>43937.291663483797</v>
+        <v>43937.291666666664</v>
       </c>
       <c r="B57">
         <v>26.16</v>
@@ -4396,7 +4387,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
-        <v>43937.333330092595</v>
+        <v>43937.333333333336</v>
       </c>
       <c r="B58">
         <v>26.4</v>
@@ -4410,7 +4401,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
-        <v>43937.374996701386</v>
+        <v>43937.375</v>
       </c>
       <c r="B59">
         <v>19.899999999999999</v>
@@ -4424,7 +4415,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
-        <v>43937.416663310185</v>
+        <v>43937.416666666664</v>
       </c>
       <c r="B60">
         <v>16.05</v>
@@ -4438,7 +4429,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
-        <v>43937.458329918984</v>
+        <v>43937.458333333336</v>
       </c>
       <c r="B61">
         <v>12.6</v>
@@ -4452,7 +4443,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
-        <v>43937.499996527775</v>
+        <v>43937.5</v>
       </c>
       <c r="B62">
         <v>11.23</v>
@@ -4466,7 +4457,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
-        <v>43937.541663136573</v>
+        <v>43937.541666666664</v>
       </c>
       <c r="B63">
         <v>9.07</v>
@@ -4480,7 +4471,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
-        <v>43937.583329745372</v>
+        <v>43937.583333333336</v>
       </c>
       <c r="B64">
         <v>7.93</v>
@@ -4494,7 +4485,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
-        <v>43937.624996354163</v>
+        <v>43937.625</v>
       </c>
       <c r="B65">
         <v>7.65</v>
@@ -4508,7 +4499,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
-        <v>43937.666662962962</v>
+        <v>43937.666666666664</v>
       </c>
       <c r="B66">
         <v>9.76</v>
@@ -4522,7 +4513,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
-        <v>43937.70832957176</v>
+        <v>43937.708333333336</v>
       </c>
       <c r="B67">
         <v>20.57</v>
@@ -4536,7 +4527,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
-        <v>43937.749996180559</v>
+        <v>43937.75</v>
       </c>
       <c r="B68">
         <v>25.7</v>
@@ -4550,7 +4541,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
-        <v>43937.79166278935</v>
+        <v>43937.791666666664</v>
       </c>
       <c r="B69">
         <v>26.19</v>
@@ -4564,7 +4555,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
-        <v>43937.833329398149</v>
+        <v>43937.833333333336</v>
       </c>
       <c r="B70">
         <v>27.59</v>
@@ -4578,7 +4569,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
-        <v>43937.874996006947</v>
+        <v>43937.875</v>
       </c>
       <c r="B71">
         <v>27.08</v>
@@ -4592,7 +4583,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
-        <v>43937.916662615738</v>
+        <v>43937.916666666664</v>
       </c>
       <c r="B72">
         <v>26.01</v>
@@ -4606,7 +4597,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
-        <v>43937.958329224537</v>
+        <v>43937.958333333336</v>
       </c>
       <c r="B73">
         <v>23.39</v>
@@ -4620,7 +4611,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
-        <v>43937.999995833336</v>
+        <v>43938</v>
       </c>
       <c r="B74">
         <v>22.02</v>
@@ -4634,7 +4625,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
-        <v>43938.041662442127</v>
+        <v>43938.041666666664</v>
       </c>
       <c r="B75">
         <v>21.09</v>
@@ -4648,7 +4639,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
-        <v>43938.083329050925</v>
+        <v>43938.083333333336</v>
       </c>
       <c r="B76">
         <v>21.04</v>
@@ -4662,7 +4653,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
-        <v>43938.124995659724</v>
+        <v>43938.125</v>
       </c>
       <c r="B77">
         <v>21.25</v>
@@ -4676,7 +4667,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
-        <v>43938.166662268515</v>
+        <v>43938.166666666664</v>
       </c>
       <c r="B78">
         <v>21.7</v>
@@ -4690,7 +4681,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
-        <v>43938.208328877314</v>
+        <v>43938.208333333336</v>
       </c>
       <c r="B79">
         <v>24.03</v>
@@ -4704,7 +4695,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
-        <v>43938.249995486112</v>
+        <v>43938.25</v>
       </c>
       <c r="B80">
         <v>26.57</v>
@@ -4718,7 +4709,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
-        <v>43938.291662094911</v>
+        <v>43938.291666666664</v>
       </c>
       <c r="B81">
         <v>26.08</v>
@@ -4732,7 +4723,7 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
-        <v>43938.333328703702</v>
+        <v>43938.333333333336</v>
       </c>
       <c r="B82">
         <v>25.95</v>
@@ -4746,7 +4737,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
-        <v>43938.374995312501</v>
+        <v>43938.375</v>
       </c>
       <c r="B83">
         <v>25.09</v>
@@ -4760,7 +4751,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
-        <v>43938.416661921299</v>
+        <v>43938.416666666664</v>
       </c>
       <c r="B84">
         <v>22.67</v>
@@ -4774,7 +4765,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
-        <v>43938.458328530091</v>
+        <v>43938.458333333336</v>
       </c>
       <c r="B85">
         <v>21.81</v>
@@ -4788,7 +4779,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
-        <v>43938.499995138889</v>
+        <v>43938.5</v>
       </c>
       <c r="B86">
         <v>20.05</v>
@@ -4802,7 +4793,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
-        <v>43938.541661747688</v>
+        <v>43938.541666666664</v>
       </c>
       <c r="B87">
         <v>18.329999999999998</v>
@@ -4816,7 +4807,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
-        <v>43938.583328356479</v>
+        <v>43938.583333333336</v>
       </c>
       <c r="B88">
         <v>18.09</v>
@@ -4830,7 +4821,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
-        <v>43938.624994965277</v>
+        <v>43938.625</v>
       </c>
       <c r="B89">
         <v>18.510000000000002</v>
@@ -4844,7 +4835,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
-        <v>43938.666661574076</v>
+        <v>43938.666666666664</v>
       </c>
       <c r="B90">
         <v>20.53</v>
@@ -4858,7 +4849,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
-        <v>43938.708328645836</v>
+        <v>43938.708333333336</v>
       </c>
       <c r="B91">
         <v>23.82</v>
@@ -4872,7 +4863,7 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
-        <v>43938.749995312501</v>
+        <v>43938.75</v>
       </c>
       <c r="B92">
         <v>26.42</v>
@@ -4886,7 +4877,7 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
-        <v>43938.791661979165</v>
+        <v>43938.791666666664</v>
       </c>
       <c r="B93">
         <v>26.45</v>
@@ -4900,7 +4891,7 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
-        <v>43938.833328645836</v>
+        <v>43938.833333333336</v>
       </c>
       <c r="B94">
         <v>27</v>
@@ -4914,7 +4905,7 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
-        <v>43938.874995312501</v>
+        <v>43938.875</v>
       </c>
       <c r="B95">
         <v>27.26</v>
@@ -4928,7 +4919,7 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
-        <v>43938.916661979165</v>
+        <v>43938.916666666664</v>
       </c>
       <c r="B96">
         <v>23.7</v>
@@ -4942,7 +4933,7 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
-        <v>43938.958328645836</v>
+        <v>43938.958333333336</v>
       </c>
       <c r="B97">
         <v>20.12</v>
@@ -4956,7 +4947,7 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
-        <v>43938.999995312501</v>
+        <v>43939</v>
       </c>
       <c r="B98">
         <v>22.05</v>
@@ -4970,7 +4961,7 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
-        <v>43939.041661979165</v>
+        <v>43939.041666666664</v>
       </c>
       <c r="B99">
         <v>21.9</v>
@@ -4984,7 +4975,7 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
-        <v>43939.083328645836</v>
+        <v>43939.083333333336</v>
       </c>
       <c r="B100">
         <v>21.47</v>
@@ -4998,7 +4989,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
-        <v>43939.124995312501</v>
+        <v>43939.125</v>
       </c>
       <c r="B101">
         <v>21.06</v>
@@ -5012,7 +5003,7 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
-        <v>43939.166661979165</v>
+        <v>43939.166666666664</v>
       </c>
       <c r="B102">
         <v>20.22</v>
@@ -5026,7 +5017,7 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
-        <v>43939.208328645836</v>
+        <v>43939.208333333336</v>
       </c>
       <c r="B103">
         <v>20.71</v>
@@ -5040,7 +5031,7 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
-        <v>43939.249995312501</v>
+        <v>43939.25</v>
       </c>
       <c r="B104">
         <v>21.16</v>
@@ -5054,7 +5045,7 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
-        <v>43939.291661979165</v>
+        <v>43939.291666666664</v>
       </c>
       <c r="B105">
         <v>22.02</v>
@@ -5068,7 +5059,7 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
-        <v>43939.333328645836</v>
+        <v>43939.333333333336</v>
       </c>
       <c r="B106">
         <v>22.55</v>
@@ -5082,7 +5073,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
-        <v>43939.374995312501</v>
+        <v>43939.375</v>
       </c>
       <c r="B107">
         <v>21.75</v>
@@ -5096,7 +5087,7 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
-        <v>43939.416661979165</v>
+        <v>43939.416666666664</v>
       </c>
       <c r="B108">
         <v>18.04</v>
@@ -5110,7 +5101,7 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
-        <v>43939.458328645836</v>
+        <v>43939.458333333336</v>
       </c>
       <c r="B109">
         <v>15.94</v>
@@ -5124,7 +5115,7 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
-        <v>43939.499995312501</v>
+        <v>43939.5</v>
       </c>
       <c r="B110">
         <v>14.84</v>
@@ -5138,7 +5129,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
-        <v>43939.541661979165</v>
+        <v>43939.541666666664</v>
       </c>
       <c r="B111">
         <v>12.5</v>
@@ -5152,7 +5143,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
-        <v>43939.583328645836</v>
+        <v>43939.583333333336</v>
       </c>
       <c r="B112">
         <v>10.43</v>
@@ -5166,7 +5157,7 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
-        <v>43939.624995312501</v>
+        <v>43939.625</v>
       </c>
       <c r="B113">
         <v>11.45</v>
@@ -5180,7 +5171,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
-        <v>43939.666661979165</v>
+        <v>43939.666666666664</v>
       </c>
       <c r="B114">
         <v>14.88</v>
@@ -5194,7 +5185,7 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
-        <v>43939.708328645836</v>
+        <v>43939.708333333336</v>
       </c>
       <c r="B115">
         <v>18.77</v>
@@ -5208,7 +5199,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
-        <v>43939.749995312501</v>
+        <v>43939.75</v>
       </c>
       <c r="B116">
         <v>23.92</v>
@@ -5222,7 +5213,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
-        <v>43939.791661979165</v>
+        <v>43939.791666666664</v>
       </c>
       <c r="B117">
         <v>23.98</v>
@@ -5236,7 +5227,7 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
-        <v>43939.833328645836</v>
+        <v>43939.833333333336</v>
       </c>
       <c r="B118">
         <v>24.46</v>
@@ -5250,7 +5241,7 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
-        <v>43939.874995312501</v>
+        <v>43939.875</v>
       </c>
       <c r="B119">
         <v>22.82</v>
@@ -5264,7 +5255,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
-        <v>43939.916661979165</v>
+        <v>43939.916666666664</v>
       </c>
       <c r="B120">
         <v>22.31</v>
@@ -5278,7 +5269,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
-        <v>43939.958328645836</v>
+        <v>43939.958333333336</v>
       </c>
       <c r="B121">
         <v>19.309999999999999</v>
@@ -5292,127 +5283,127 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
-        <v>43939.999995312501</v>
+        <v>43940</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
-        <v>43940.041661979165</v>
+        <v>43940.041666666664</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
-        <v>43940.083328645836</v>
+        <v>43940.083333333336</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
-        <v>43940.124995312501</v>
+        <v>43940.125</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
-        <v>43940.166661979165</v>
+        <v>43940.166666666664</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
-        <v>43940.208328645836</v>
+        <v>43940.208333333336</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
-        <v>43940.249995312501</v>
+        <v>43940.25</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
-        <v>43940.291661979165</v>
+        <v>43940.291666666664</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
-        <v>43940.333328645836</v>
+        <v>43940.333333333336</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
-        <v>43940.374995312501</v>
+        <v>43940.375</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
-        <v>43940.416661979165</v>
+        <v>43940.416666666664</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
-        <v>43940.458328645836</v>
+        <v>43940.458333333336</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
-        <v>43940.499995312501</v>
+        <v>43940.5</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
-        <v>43940.541661979165</v>
+        <v>43940.541666666664</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
-        <v>43940.583328645836</v>
+        <v>43940.583333333336</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
-        <v>43940.624995312501</v>
+        <v>43940.625</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
-        <v>43940.666661979165</v>
+        <v>43940.666666666664</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
-        <v>43940.708328645836</v>
+        <v>43940.708333333336</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
-        <v>43940.749995312501</v>
+        <v>43940.75</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
-        <v>43940.791661979165</v>
+        <v>43940.791666666664</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
-        <v>43940.833328645836</v>
+        <v>43940.833333333336</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
-        <v>43940.874995312501</v>
+        <v>43940.875</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
-        <v>43940.916661979165</v>
+        <v>43940.916666666664</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
-        <v>43940.958328645836</v>
+        <v>43940.958333333336</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
-        <v>43940.999995312501</v>
+        <v>43941</v>
       </c>
       <c r="B146">
         <v>8.4700000000000006</v>
@@ -5426,7 +5417,7 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
-        <v>43941.041661979165</v>
+        <v>43941.041666666664</v>
       </c>
       <c r="B147">
         <v>6.49</v>
@@ -5440,7 +5431,7 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
-        <v>43941.083328645836</v>
+        <v>43941.083333333336</v>
       </c>
       <c r="B148">
         <v>4.67</v>
@@ -5454,7 +5445,7 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
-        <v>43941.124995312501</v>
+        <v>43941.125</v>
       </c>
       <c r="B149">
         <v>3.98</v>
@@ -5468,7 +5459,7 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
-        <v>43941.166661979165</v>
+        <v>43941.166666666664</v>
       </c>
       <c r="B150">
         <v>4.17</v>
@@ -5482,7 +5473,7 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
-        <v>43941.208328645836</v>
+        <v>43941.208333333336</v>
       </c>
       <c r="B151">
         <v>9.02</v>
@@ -5496,7 +5487,7 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
-        <v>43941.249995312501</v>
+        <v>43941.25</v>
       </c>
       <c r="B152">
         <v>18.940000000000001</v>
@@ -5510,7 +5501,7 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
-        <v>43941.291661979165</v>
+        <v>43941.291666666664</v>
       </c>
       <c r="B153">
         <v>22.37</v>
@@ -5524,7 +5515,7 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
-        <v>43941.333328645836</v>
+        <v>43941.333333333336</v>
       </c>
       <c r="B154">
         <v>21.94</v>
@@ -5538,7 +5529,7 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
-        <v>43941.374995312501</v>
+        <v>43941.375</v>
       </c>
       <c r="B155">
         <v>14.94</v>
@@ -5552,7 +5543,7 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
-        <v>43941.416661979165</v>
+        <v>43941.416666666664</v>
       </c>
       <c r="B156">
         <v>13.52</v>
@@ -5566,7 +5557,7 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
-        <v>43941.458328645836</v>
+        <v>43941.458333333336</v>
       </c>
       <c r="B157">
         <v>13.5</v>
@@ -5580,7 +5571,7 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
-        <v>43941.499995312501</v>
+        <v>43941.5</v>
       </c>
       <c r="B158">
         <v>9.08</v>
@@ -5594,7 +5585,7 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
-        <v>43941.541661979165</v>
+        <v>43941.541666666664</v>
       </c>
       <c r="B159">
         <v>6.24</v>
@@ -5608,7 +5599,7 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
-        <v>43941.583328645836</v>
+        <v>43941.583333333336</v>
       </c>
       <c r="B160">
         <v>0.79</v>
@@ -5622,7 +5613,7 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
-        <v>43941.624995312501</v>
+        <v>43941.625</v>
       </c>
       <c r="B161">
         <v>0.02</v>
@@ -5636,7 +5627,7 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
-        <v>43941.666661979165</v>
+        <v>43941.666666666664</v>
       </c>
       <c r="B162">
         <v>1.01</v>
@@ -5650,7 +5641,7 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
-        <v>43941.708328645836</v>
+        <v>43941.708333333336</v>
       </c>
       <c r="B163">
         <v>12.84</v>
@@ -5664,7 +5655,7 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
-        <v>43941.749995312501</v>
+        <v>43941.75</v>
       </c>
       <c r="B164">
         <v>15.13</v>
@@ -5678,7 +5669,7 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
-        <v>43941.791661979165</v>
+        <v>43941.791666666664</v>
       </c>
       <c r="B165">
         <v>20.41</v>
@@ -5692,7 +5683,7 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
-        <v>43941.833328645836</v>
+        <v>43941.833333333336</v>
       </c>
       <c r="B166">
         <v>21.6</v>
@@ -5706,7 +5697,7 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
-        <v>43941.874995312501</v>
+        <v>43941.875</v>
       </c>
       <c r="B167">
         <v>18.670000000000002</v>
@@ -5720,7 +5711,7 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
-        <v>43941.916661979165</v>
+        <v>43941.916666666664</v>
       </c>
       <c r="B168">
         <v>15</v>
@@ -5734,7 +5725,7 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
-        <v>43941.958328645836</v>
+        <v>43941.958333333336</v>
       </c>
       <c r="B169">
         <v>13.19</v>
@@ -5748,7 +5739,7 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
-        <v>43941.999995312501</v>
+        <v>43942</v>
       </c>
       <c r="B170">
         <v>4.72</v>
@@ -5762,7 +5753,7 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
-        <v>43942.041661979165</v>
+        <v>43942.041666666664</v>
       </c>
       <c r="B171">
         <v>4.29</v>
@@ -5776,7 +5767,7 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
-        <v>43942.083328645836</v>
+        <v>43942.083333333336</v>
       </c>
       <c r="B172">
         <v>1.28</v>
@@ -5790,7 +5781,7 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
-        <v>43942.124995312501</v>
+        <v>43942.125</v>
       </c>
       <c r="B173">
         <v>-1.89</v>
@@ -5804,7 +5795,7 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
-        <v>43942.166661979165</v>
+        <v>43942.166666666664</v>
       </c>
       <c r="B174">
         <v>-0.61</v>
@@ -5818,7 +5809,7 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
-        <v>43942.208328645836</v>
+        <v>43942.208333333336</v>
       </c>
       <c r="B175">
         <v>8.2799999999999994</v>
@@ -5832,7 +5823,7 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
-        <v>43942.249995312501</v>
+        <v>43942.25</v>
       </c>
       <c r="B176">
         <v>13.68</v>
@@ -5846,7 +5837,7 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
-        <v>43942.291661979165</v>
+        <v>43942.291666666664</v>
       </c>
       <c r="B177">
         <v>17.28</v>
@@ -5860,7 +5851,7 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
-        <v>43942.333328645836</v>
+        <v>43942.333333333336</v>
       </c>
       <c r="B178">
         <v>17.03</v>
@@ -5874,7 +5865,7 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
-        <v>43942.374995312501</v>
+        <v>43942.375</v>
       </c>
       <c r="B179">
         <v>14.68</v>
@@ -5888,7 +5879,7 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
-        <v>43942.416661979165</v>
+        <v>43942.416666666664</v>
       </c>
       <c r="B180">
         <v>13.24</v>
@@ -5902,7 +5893,7 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
-        <v>43942.458328645836</v>
+        <v>43942.458333333336</v>
       </c>
       <c r="B181">
         <v>14.69</v>
@@ -5916,7 +5907,7 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
-        <v>43942.499995312501</v>
+        <v>43942.5</v>
       </c>
       <c r="B182">
         <v>12.94</v>
@@ -5930,7 +5921,7 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
-        <v>43942.541661979165</v>
+        <v>43942.541666666664</v>
       </c>
       <c r="B183">
         <v>13.5</v>
@@ -5944,7 +5935,7 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
-        <v>43942.583328645836</v>
+        <v>43942.583333333336</v>
       </c>
       <c r="B184">
         <v>13.92</v>
@@ -5958,7 +5949,7 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
-        <v>43942.624995312501</v>
+        <v>43942.625</v>
       </c>
       <c r="B185">
         <v>8.6199999999999992</v>
@@ -5972,7 +5963,7 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
-        <v>43942.666661979165</v>
+        <v>43942.666666666664</v>
       </c>
       <c r="B186">
         <v>9.9</v>
@@ -5986,7 +5977,7 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
-        <v>43942.708328645836</v>
+        <v>43942.708333333336</v>
       </c>
       <c r="B187">
         <v>11.5</v>
@@ -6000,7 +5991,7 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
-        <v>43942.749995312501</v>
+        <v>43942.75</v>
       </c>
       <c r="B188">
         <v>13.86</v>
@@ -6014,7 +6005,7 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
-        <v>43942.791661979165</v>
+        <v>43942.791666666664</v>
       </c>
       <c r="B189">
         <v>15.2</v>
@@ -6028,7 +6019,7 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
-        <v>43942.833328645836</v>
+        <v>43942.833333333336</v>
       </c>
       <c r="B190">
         <v>16.46</v>
@@ -6042,7 +6033,7 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
-        <v>43942.874995312501</v>
+        <v>43942.875</v>
       </c>
       <c r="B191">
         <v>13.01</v>
@@ -6056,7 +6047,7 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
-        <v>43942.916661979165</v>
+        <v>43942.916666666664</v>
       </c>
       <c r="B192">
         <v>13.69</v>
@@ -6070,7 +6061,7 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
-        <v>43942.958328645836</v>
+        <v>43942.958333333336</v>
       </c>
       <c r="B193">
         <v>9.07</v>
@@ -6084,7 +6075,7 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
-        <v>43942.999995312501</v>
+        <v>43943</v>
       </c>
       <c r="B194">
         <v>8.08</v>
@@ -6098,7 +6089,7 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
-        <v>43943.041661979165</v>
+        <v>43943.041666666664</v>
       </c>
       <c r="B195">
         <v>6.85</v>
@@ -6112,7 +6103,7 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
-        <v>43943.083328645836</v>
+        <v>43943.083333333336</v>
       </c>
       <c r="B196">
         <v>6.42</v>
@@ -6126,7 +6117,7 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
-        <v>43943.124995312501</v>
+        <v>43943.125</v>
       </c>
       <c r="B197">
         <v>5.87</v>
@@ -6140,7 +6131,7 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
-        <v>43943.166661979165</v>
+        <v>43943.166666666664</v>
       </c>
       <c r="B198">
         <v>7.33</v>
@@ -6154,7 +6145,7 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
-        <v>43943.208328645836</v>
+        <v>43943.208333333336</v>
       </c>
       <c r="B199">
         <v>8.27</v>
@@ -6168,7 +6159,7 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
-        <v>43943.249995312501</v>
+        <v>43943.25</v>
       </c>
       <c r="B200">
         <v>16.690000000000001</v>
@@ -6182,7 +6173,7 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
-        <v>43943.291661979165</v>
+        <v>43943.291666666664</v>
       </c>
       <c r="B201">
         <v>20.67</v>
@@ -6196,7 +6187,7 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
-        <v>43943.333328645836</v>
+        <v>43943.333333333336</v>
       </c>
       <c r="B202">
         <v>21</v>
@@ -6210,7 +6201,7 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
-        <v>43943.374995312501</v>
+        <v>43943.375</v>
       </c>
       <c r="B203">
         <v>15.07</v>
@@ -6224,7 +6215,7 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
-        <v>43943.416661979165</v>
+        <v>43943.416666666664</v>
       </c>
       <c r="B204">
         <v>9.09</v>
@@ -6238,7 +6229,7 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
-        <v>43943.458328645836</v>
+        <v>43943.458333333336</v>
       </c>
       <c r="B205">
         <v>6.74</v>
@@ -6252,7 +6243,7 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
-        <v>43943.499995312501</v>
+        <v>43943.5</v>
       </c>
       <c r="B206">
         <v>6.68</v>
@@ -6266,7 +6257,7 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
-        <v>43943.541661979165</v>
+        <v>43943.541666666664</v>
       </c>
       <c r="B207">
         <v>4.67</v>
@@ -6280,7 +6271,7 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
-        <v>43943.583328645836</v>
+        <v>43943.583333333336</v>
       </c>
       <c r="B208">
         <v>0.94</v>
@@ -6294,7 +6285,7 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
-        <v>43943.624995312501</v>
+        <v>43943.625</v>
       </c>
       <c r="B209">
         <v>1.62</v>
@@ -6308,7 +6299,7 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
-        <v>43943.666661979165</v>
+        <v>43943.666666666664</v>
       </c>
       <c r="B210">
         <v>5.82</v>
@@ -6322,7 +6313,7 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
-        <v>43943.708328645836</v>
+        <v>43943.708333333336</v>
       </c>
       <c r="B211">
         <v>11.16</v>
@@ -6336,7 +6327,7 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
-        <v>43943.749995312501</v>
+        <v>43943.75</v>
       </c>
       <c r="B212">
         <v>19.47</v>
@@ -6350,7 +6341,7 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
-        <v>43943.791661979165</v>
+        <v>43943.791666666664</v>
       </c>
       <c r="B213">
         <v>22.37</v>
@@ -6364,7 +6355,7 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
-        <v>43943.833328645836</v>
+        <v>43943.833333333336</v>
       </c>
       <c r="B214">
         <v>23.19</v>
@@ -6378,7 +6369,7 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
-        <v>43943.874995312501</v>
+        <v>43943.875</v>
       </c>
       <c r="B215">
         <v>20.67</v>
@@ -6392,7 +6383,7 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
-        <v>43943.916661979165</v>
+        <v>43943.916666666664</v>
       </c>
       <c r="B216">
         <v>19.57</v>
@@ -6406,7 +6397,7 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
-        <v>43943.958328645836</v>
+        <v>43943.958333333336</v>
       </c>
       <c r="B217">
         <v>17.670000000000002</v>
@@ -6420,7 +6411,7 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
-        <v>43943.999995312501</v>
+        <v>43944</v>
       </c>
       <c r="B218">
         <v>20.09</v>
@@ -6434,7 +6425,7 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
-        <v>43944.041661979165</v>
+        <v>43944.041666666664</v>
       </c>
       <c r="B219">
         <v>18.34</v>
@@ -6448,7 +6439,7 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
-        <v>43944.083328645836</v>
+        <v>43944.083333333336</v>
       </c>
       <c r="B220">
         <v>18.3</v>
@@ -6462,7 +6453,7 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
-        <v>43944.124995312501</v>
+        <v>43944.125</v>
       </c>
       <c r="B221">
         <v>18.57</v>
@@ -6476,7 +6467,7 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
-        <v>43944.166661979165</v>
+        <v>43944.166666666664</v>
       </c>
       <c r="B222">
         <v>18.48</v>
@@ -6490,7 +6481,7 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
-        <v>43944.208328645836</v>
+        <v>43944.208333333336</v>
       </c>
       <c r="B223">
         <v>19.84</v>
@@ -6504,7 +6495,7 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
-        <v>43944.249995312501</v>
+        <v>43944.25</v>
       </c>
       <c r="B224">
         <v>24.59</v>
@@ -6518,7 +6509,7 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
-        <v>43944.291661979165</v>
+        <v>43944.291666666664</v>
       </c>
       <c r="B225">
         <v>21.9</v>
@@ -6532,7 +6523,7 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
-        <v>43944.333328645836</v>
+        <v>43944.333333333336</v>
       </c>
       <c r="B226">
         <v>22</v>
@@ -6546,7 +6537,7 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
-        <v>43944.374995312501</v>
+        <v>43944.375</v>
       </c>
       <c r="B227">
         <v>19.59</v>
@@ -6560,7 +6551,7 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
-        <v>43944.416661979165</v>
+        <v>43944.416666666664</v>
       </c>
       <c r="B228">
         <v>18.82</v>
@@ -6574,7 +6565,7 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
-        <v>43944.458328645836</v>
+        <v>43944.458333333336</v>
       </c>
       <c r="B229">
         <v>19.13</v>
@@ -6588,7 +6579,7 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
-        <v>43944.499995312501</v>
+        <v>43944.5</v>
       </c>
       <c r="B230">
         <v>17.59</v>
@@ -6602,7 +6593,7 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
-        <v>43944.541661979165</v>
+        <v>43944.541666666664</v>
       </c>
       <c r="B231">
         <v>16.79</v>
@@ -6616,7 +6607,7 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
-        <v>43944.583328645836</v>
+        <v>43944.583333333336</v>
       </c>
       <c r="B232">
         <v>15.01</v>
@@ -6630,7 +6621,7 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
-        <v>43944.624995312501</v>
+        <v>43944.625</v>
       </c>
       <c r="B233">
         <v>15.02</v>
@@ -6644,7 +6635,7 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
-        <v>43944.666661979165</v>
+        <v>43944.666666666664</v>
       </c>
       <c r="B234">
         <v>15.54</v>
@@ -6658,7 +6649,7 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
-        <v>43944.708328645836</v>
+        <v>43944.708333333336</v>
       </c>
       <c r="B235">
         <v>19.09</v>
@@ -6672,7 +6663,7 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
-        <v>43944.749995312501</v>
+        <v>43944.75</v>
       </c>
       <c r="B236">
         <v>20.99</v>
@@ -6686,7 +6677,7 @@
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
-        <v>43944.791661979165</v>
+        <v>43944.791666666664</v>
       </c>
       <c r="B237">
         <v>20.04</v>
@@ -6700,7 +6691,7 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A238" s="1">
-        <v>43944.833328645836</v>
+        <v>43944.833333333336</v>
       </c>
       <c r="B238">
         <v>22.26</v>
@@ -6714,7 +6705,7 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
-        <v>43944.874995312501</v>
+        <v>43944.875</v>
       </c>
       <c r="B239">
         <v>24.71</v>
@@ -6728,7 +6719,7 @@
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
-        <v>43944.916661979165</v>
+        <v>43944.916666666664</v>
       </c>
       <c r="B240">
         <v>24.32</v>
@@ -6742,7 +6733,7 @@
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
-        <v>43944.958328645836</v>
+        <v>43944.958333333336</v>
       </c>
       <c r="B241">
         <v>21.38</v>
@@ -6756,7 +6747,7 @@
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
-        <v>43944.999995312501</v>
+        <v>43945</v>
       </c>
       <c r="B242">
         <v>23.76</v>
@@ -6770,7 +6761,7 @@
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
-        <v>43945.041661979165</v>
+        <v>43945.041666666664</v>
       </c>
       <c r="B243">
         <v>22.57</v>
@@ -6784,7 +6775,7 @@
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
-        <v>43945.083328645836</v>
+        <v>43945.083333333336</v>
       </c>
       <c r="B244">
         <v>21.24</v>
@@ -6798,7 +6789,7 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
-        <v>43945.124995312501</v>
+        <v>43945.125</v>
       </c>
       <c r="B245">
         <v>20.47</v>
@@ -6812,7 +6803,7 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
-        <v>43945.166661979165</v>
+        <v>43945.166666666664</v>
       </c>
       <c r="B246">
         <v>20.54</v>
@@ -6826,7 +6817,7 @@
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
-        <v>43945.208328645836</v>
+        <v>43945.208333333336</v>
       </c>
       <c r="B247">
         <v>21.39</v>
@@ -6840,7 +6831,7 @@
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
-        <v>43945.249995312501</v>
+        <v>43945.25</v>
       </c>
       <c r="B248">
         <v>26.11</v>
@@ -6854,7 +6845,7 @@
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
-        <v>43945.291661979165</v>
+        <v>43945.291666666664</v>
       </c>
       <c r="B249">
         <v>24.62</v>
@@ -6868,7 +6859,7 @@
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
-        <v>43945.333328645836</v>
+        <v>43945.333333333336</v>
       </c>
       <c r="B250">
         <v>26.56</v>
@@ -6882,7 +6873,7 @@
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
-        <v>43945.374995312501</v>
+        <v>43945.375</v>
       </c>
       <c r="B251">
         <v>22.03</v>
@@ -6896,7 +6887,7 @@
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
-        <v>43945.416661979165</v>
+        <v>43945.416666666664</v>
       </c>
       <c r="B252">
         <v>16.059999999999999</v>
@@ -6910,7 +6901,7 @@
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A253" s="1">
-        <v>43945.458328645836</v>
+        <v>43945.458333333336</v>
       </c>
       <c r="B253">
         <v>14.05</v>
@@ -6924,7 +6915,7 @@
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A254" s="1">
-        <v>43945.499995312501</v>
+        <v>43945.5</v>
       </c>
       <c r="B254">
         <v>12.76</v>
@@ -6938,7 +6929,7 @@
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
-        <v>43945.541661979165</v>
+        <v>43945.541666666664</v>
       </c>
       <c r="B255">
         <v>9.0399999999999991</v>
@@ -6952,7 +6943,7 @@
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
-        <v>43945.583328645836</v>
+        <v>43945.583333333336</v>
       </c>
       <c r="B256">
         <v>5.0999999999999996</v>
@@ -6966,7 +6957,7 @@
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
-        <v>43945.624995312501</v>
+        <v>43945.625</v>
       </c>
       <c r="B257">
         <v>4.3</v>
@@ -6980,7 +6971,7 @@
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
-        <v>43945.666661979165</v>
+        <v>43945.666666666664</v>
       </c>
       <c r="B258">
         <v>7.04</v>
@@ -6994,7 +6985,7 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
-        <v>43945.708328645836</v>
+        <v>43945.708333333336</v>
       </c>
       <c r="B259">
         <v>12.31</v>
@@ -7008,7 +6999,7 @@
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A260" s="1">
-        <v>43945.749995312501</v>
+        <v>43945.75</v>
       </c>
       <c r="B260">
         <v>15.61</v>
@@ -7022,7 +7013,7 @@
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A261" s="1">
-        <v>43945.791661979165</v>
+        <v>43945.791666666664</v>
       </c>
       <c r="B261">
         <v>20.260000000000002</v>
@@ -7036,7 +7027,7 @@
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A262" s="1">
-        <v>43945.833328645836</v>
+        <v>43945.833333333336</v>
       </c>
       <c r="B262">
         <v>21.03</v>
@@ -7050,7 +7041,7 @@
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A263" s="1">
-        <v>43945.874995312501</v>
+        <v>43945.875</v>
       </c>
       <c r="B263">
         <v>19.7</v>
@@ -7064,7 +7055,7 @@
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A264" s="1">
-        <v>43945.916661979165</v>
+        <v>43945.916666666664</v>
       </c>
       <c r="B264">
         <v>18.47</v>
@@ -7078,7 +7069,7 @@
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A265" s="1">
-        <v>43945.958328645836</v>
+        <v>43945.958333333336</v>
       </c>
       <c r="B265">
         <v>16.7</v>
@@ -7092,7 +7083,7 @@
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A266" s="1">
-        <v>43945.999995312501</v>
+        <v>43946</v>
       </c>
       <c r="B266">
         <v>14.96</v>
@@ -7106,7 +7097,7 @@
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A267" s="1">
-        <v>43946.041661979165</v>
+        <v>43946.041666666664</v>
       </c>
       <c r="B267">
         <v>14.13</v>
@@ -7120,7 +7111,7 @@
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A268" s="1">
-        <v>43946.083328645836</v>
+        <v>43946.083333333336</v>
       </c>
       <c r="B268">
         <v>13.34</v>
@@ -7134,7 +7125,7 @@
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A269" s="1">
-        <v>43946.124995312501</v>
+        <v>43946.125</v>
       </c>
       <c r="B269">
         <v>12.94</v>
@@ -7148,7 +7139,7 @@
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A270" s="1">
-        <v>43946.166661979165</v>
+        <v>43946.166666666664</v>
       </c>
       <c r="B270">
         <v>12.4</v>
@@ -7162,7 +7153,7 @@
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A271" s="1">
-        <v>43946.208328645836</v>
+        <v>43946.208333333336</v>
       </c>
       <c r="B271">
         <v>13.04</v>
@@ -7176,7 +7167,7 @@
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A272" s="1">
-        <v>43946.249995543978</v>
+        <v>43946.25</v>
       </c>
       <c r="B272">
         <v>14.67</v>
@@ -7190,7 +7181,7 @@
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A273" s="1">
-        <v>43946.291662268515</v>
+        <v>43946.291666666664</v>
       </c>
       <c r="B273">
         <v>18</v>
@@ -7204,7 +7195,7 @@
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A274" s="1">
-        <v>43946.333328993052</v>
+        <v>43946.333333333336</v>
       </c>
       <c r="B274">
         <v>19.57</v>
@@ -7218,7 +7209,7 @@
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A275" s="1">
-        <v>43946.37499571759</v>
+        <v>43946.375</v>
       </c>
       <c r="B275">
         <v>16.22</v>
@@ -7232,7 +7223,7 @@
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A276" s="1">
-        <v>43946.416662442127</v>
+        <v>43946.416666666664</v>
       </c>
       <c r="B276">
         <v>13.47</v>
@@ -7246,7 +7237,7 @@
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A277" s="1">
-        <v>43946.458329166664</v>
+        <v>43946.458333333336</v>
       </c>
       <c r="B277">
         <v>12.9</v>
@@ -7260,7 +7251,7 @@
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A278" s="1">
-        <v>43946.499995891201</v>
+        <v>43946.5</v>
       </c>
       <c r="B278">
         <v>11.92</v>
@@ -7274,7 +7265,7 @@
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A279" s="1">
-        <v>43946.541662615738</v>
+        <v>43946.541666666664</v>
       </c>
       <c r="B279">
         <v>9.59</v>
@@ -7288,7 +7279,7 @@
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A280" s="1">
-        <v>43946.583329340276</v>
+        <v>43946.583333333336</v>
       </c>
       <c r="B280">
         <v>8.02</v>
@@ -7302,7 +7293,7 @@
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A281" s="1">
-        <v>43946.624996064813</v>
+        <v>43946.625</v>
       </c>
       <c r="B281">
         <v>9.08</v>
@@ -7316,7 +7307,7 @@
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A282" s="1">
-        <v>43946.66666278935</v>
+        <v>43946.666666666664</v>
       </c>
       <c r="B282">
         <v>13.76</v>
@@ -7330,7 +7321,7 @@
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A283" s="1">
-        <v>43946.708329513887</v>
+        <v>43946.708333333336</v>
       </c>
       <c r="B283">
         <v>19.25</v>
@@ -7344,7 +7335,7 @@
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A284" s="1">
-        <v>43946.749996238425</v>
+        <v>43946.75</v>
       </c>
       <c r="B284">
         <v>21.57</v>
@@ -7358,7 +7349,7 @@
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A285" s="1">
-        <v>43946.791662962962</v>
+        <v>43946.791666666664</v>
       </c>
       <c r="B285">
         <v>21.12</v>
@@ -7372,7 +7363,7 @@
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A286" s="1">
-        <v>43946.833329687499</v>
+        <v>43946.833333333336</v>
       </c>
       <c r="B286">
         <v>21.96</v>
@@ -7386,7 +7377,7 @@
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A287" s="1">
-        <v>43946.874996412036</v>
+        <v>43946.875</v>
       </c>
       <c r="B287">
         <v>22.39</v>
@@ -7400,7 +7391,7 @@
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A288" s="1">
-        <v>43946.916663136573</v>
+        <v>43946.916666666664</v>
       </c>
       <c r="B288">
         <v>22.92</v>
@@ -7414,7 +7405,7 @@
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A289" s="1">
-        <v>43946.958329861111</v>
+        <v>43946.958333333336</v>
       </c>
       <c r="B289">
         <v>21.17</v>
@@ -7424,6 +7415,342 @@
       </c>
       <c r="D289">
         <v>21.23</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A290" s="1">
+        <v>43947</v>
+      </c>
+      <c r="B290">
+        <v>18.02</v>
+      </c>
+      <c r="C290">
+        <v>22.3</v>
+      </c>
+      <c r="D290">
+        <v>16.23</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A291" s="1">
+        <v>43947.041666666664</v>
+      </c>
+      <c r="B291">
+        <v>16.32</v>
+      </c>
+      <c r="C291">
+        <v>19.79</v>
+      </c>
+      <c r="D291">
+        <v>15.76</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A292" s="1">
+        <v>43947.083333333336</v>
+      </c>
+      <c r="B292">
+        <v>15.26</v>
+      </c>
+      <c r="C292">
+        <v>20.76</v>
+      </c>
+      <c r="D292">
+        <v>14.55</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A293" s="1">
+        <v>43947.125</v>
+      </c>
+      <c r="B293">
+        <v>15.21</v>
+      </c>
+      <c r="C293">
+        <v>21.06</v>
+      </c>
+      <c r="D293">
+        <v>12.42</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A294" s="1">
+        <v>43947.166666666664</v>
+      </c>
+      <c r="B294">
+        <v>15.06</v>
+      </c>
+      <c r="C294">
+        <v>22.23</v>
+      </c>
+      <c r="D294">
+        <v>11.92</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A295" s="1">
+        <v>43947.208333333336</v>
+      </c>
+      <c r="B295">
+        <v>15.2</v>
+      </c>
+      <c r="C295">
+        <v>21.95</v>
+      </c>
+      <c r="D295">
+        <v>11.8</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A296" s="1">
+        <v>43947.25</v>
+      </c>
+      <c r="B296">
+        <v>15.2</v>
+      </c>
+      <c r="C296">
+        <v>18.809999999999999</v>
+      </c>
+      <c r="D296">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A297" s="1">
+        <v>43947.291666666664</v>
+      </c>
+      <c r="B297">
+        <v>14.89</v>
+      </c>
+      <c r="C297">
+        <v>18.09</v>
+      </c>
+      <c r="D297">
+        <v>11.99</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A298" s="1">
+        <v>43947.333333333336</v>
+      </c>
+      <c r="B298">
+        <v>14.42</v>
+      </c>
+      <c r="C298">
+        <v>16.059999999999999</v>
+      </c>
+      <c r="D298">
+        <v>12.12</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A299" s="1">
+        <v>43947.375</v>
+      </c>
+      <c r="B299">
+        <v>14.51</v>
+      </c>
+      <c r="C299">
+        <v>15.01</v>
+      </c>
+      <c r="D299">
+        <v>12.42</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A300" s="1">
+        <v>43947.416666666664</v>
+      </c>
+      <c r="B300">
+        <v>11.94</v>
+      </c>
+      <c r="C300">
+        <v>13</v>
+      </c>
+      <c r="D300">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A301" s="1">
+        <v>43947.458333333336</v>
+      </c>
+      <c r="B301">
+        <v>12.03</v>
+      </c>
+      <c r="C301">
+        <v>14.38</v>
+      </c>
+      <c r="D301">
+        <v>14.38</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A302" s="1">
+        <v>43947.5</v>
+      </c>
+      <c r="B302">
+        <v>10.59</v>
+      </c>
+      <c r="C302">
+        <v>15</v>
+      </c>
+      <c r="D302">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A303" s="1">
+        <v>43947.541666666664</v>
+      </c>
+      <c r="B303">
+        <v>9.01</v>
+      </c>
+      <c r="C303">
+        <v>11.9</v>
+      </c>
+      <c r="D303">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A304" s="1">
+        <v>43947.583333333336</v>
+      </c>
+      <c r="B304">
+        <v>5.81</v>
+      </c>
+      <c r="C304">
+        <v>5.56</v>
+      </c>
+      <c r="D304">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A305" s="1">
+        <v>43947.625</v>
+      </c>
+      <c r="B305">
+        <v>5.61</v>
+      </c>
+      <c r="C305">
+        <v>6.93</v>
+      </c>
+      <c r="D305">
+        <v>6.93</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A306" s="1">
+        <v>43947.666666666664</v>
+      </c>
+      <c r="B306">
+        <v>7.9</v>
+      </c>
+      <c r="C306">
+        <v>12.42</v>
+      </c>
+      <c r="D306">
+        <v>12.42</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A307" s="1">
+        <v>43947.708333333336</v>
+      </c>
+      <c r="B307">
+        <v>15.13</v>
+      </c>
+      <c r="C307">
+        <v>16.149999999999999</v>
+      </c>
+      <c r="D307">
+        <v>12.42</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A308" s="1">
+        <v>43947.75</v>
+      </c>
+      <c r="B308">
+        <v>23.73</v>
+      </c>
+      <c r="C308">
+        <v>24.82</v>
+      </c>
+      <c r="D308">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A309" s="1">
+        <v>43947.791666666664</v>
+      </c>
+      <c r="B309">
+        <v>23.97</v>
+      </c>
+      <c r="C309">
+        <v>27.97</v>
+      </c>
+      <c r="D309">
+        <v>17.07</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A310" s="1">
+        <v>43947.833333333336</v>
+      </c>
+      <c r="B310">
+        <v>24.83</v>
+      </c>
+      <c r="C310">
+        <v>31.84</v>
+      </c>
+      <c r="D310">
+        <v>19.46</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A311" s="1">
+        <v>43947.875</v>
+      </c>
+      <c r="B311">
+        <v>24.96</v>
+      </c>
+      <c r="C311">
+        <v>27.49</v>
+      </c>
+      <c r="D311">
+        <v>24.1</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A312" s="1">
+        <v>43947.916666666664</v>
+      </c>
+      <c r="B312">
+        <v>25.66</v>
+      </c>
+      <c r="C312">
+        <v>26.06</v>
+      </c>
+      <c r="D312">
+        <v>25.15</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A313" s="1">
+        <v>43947.958333333336</v>
+      </c>
+      <c r="B313">
+        <v>23.59</v>
+      </c>
+      <c r="C313">
+        <v>23.76</v>
+      </c>
+      <c r="D313">
+        <v>23.76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>